<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-study-summary-ig@1a0969d978181d3e5d487c5b2dfd9437a9add4fa 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-study-summary.xlsx
+++ b/StructureDefinition-study-summary.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-04-08T19:05:18+00:00</t>
+    <t>2022-04-11T21:19:38+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -770,7 +770,7 @@
     <t>Observation.subject</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Group)
+    <t xml:space="preserve">Reference(https://ncpi-fhir.github.io/ncpi-fhir-study-summary-ig/StructureDefinition/study-summary-group)
 </t>
   </si>
   <si>
@@ -801,7 +801,7 @@
     <t>Observation.focus</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(ResearchStudy)
+    <t xml:space="preserve">Reference(https://ncpi-fhir.github.io/ncpi-fhir-study-summary-ig/StructureDefinition/summary-research-study)
 </t>
   </si>
   <si>

</xml_diff>